<commit_message>
Update mekanisme promo gabungan
</commit_message>
<xml_diff>
--- a/aturan_promo.xlsx
+++ b/aturan_promo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.133\ina\2022\SPV TM (Nur)\Optimalisasi\Node\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\promo-calculation\promo-calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43BF815-F59C-4AB6-83E4-54F21D058096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE0CA64-97EC-4916-B4D0-27DA9CEE1D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B916ECD5-1FA5-4E80-A6F9-92B25007873D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B916ECD5-1FA5-4E80-A6F9-92B25007873D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,40 +140,40 @@
     <t>Ya</t>
   </si>
   <si>
-    <t>Top 4</t>
-  </si>
-  <si>
     <t>Gabungan Kuantitas</t>
   </si>
   <si>
-    <t>Gabungan Values</t>
-  </si>
-  <si>
     <t>FORTIUS 10|GOODBIS 21</t>
   </si>
   <si>
     <t>OKEBIS CHOCOLATE COOKIES 28|OKEBIS KELAPA EXTRA 28|OKEBIS COOKIES CREAM 72</t>
   </si>
   <si>
-    <t>Gabungan 1</t>
-  </si>
-  <si>
     <t>FORTIUS 30|OKEBIS KELAPA CREAM 28</t>
   </si>
   <si>
-    <t>Gabungan 2</t>
-  </si>
-  <si>
-    <t>Gabungan 3</t>
-  </si>
-  <si>
-    <t>Gabungan 4</t>
-  </si>
-  <si>
-    <t>Gabungan 5</t>
-  </si>
-  <si>
     <t>OKEBIS KELAPA EXTRA 28|OKEBIS KELAPA CREAM 28</t>
+  </si>
+  <si>
+    <t>Kelompok_1</t>
+  </si>
+  <si>
+    <t>Kelompok_2</t>
+  </si>
+  <si>
+    <t>Kelompok_3</t>
+  </si>
+  <si>
+    <t>Kelompok_4</t>
+  </si>
+  <si>
+    <t>Gabungan Value</t>
+  </si>
+  <si>
+    <t>Kelompok_5</t>
+  </si>
+  <si>
+    <t>GOODBIS 21|OKEBIS CHOCOCHIPS COOKIES 48</t>
   </si>
 </sst>
 </file>
@@ -550,21 +550,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE55C23-1BA9-40E7-8EA2-0FEACD3BFDA1}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -593,7 +595,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -616,10 +618,10 @@
         <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -642,10 +644,10 @@
         <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -668,18 +670,18 @@
         <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1">
         <v>6</v>
@@ -694,21 +696,21 @@
         <v>32</v>
       </c>
       <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
       </c>
       <c r="D6" s="1">
         <v>10</v>
@@ -723,21 +725,21 @@
         <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1">
         <v>300000</v>
@@ -752,79 +754,79 @@
         <v>32</v>
       </c>
       <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="I7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
       <c r="D8" s="1">
-        <v>200000</v>
+        <v>300000</v>
       </c>
       <c r="E8" s="1">
         <v>999999</v>
       </c>
       <c r="F8">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1">
-        <v>300000</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1">
         <v>999999</v>
       </c>
       <c r="F9">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="I9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1">
         <v>200000</v>
@@ -845,15 +847,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1">
         <v>200000</v>
@@ -868,13 +870,13 @@
         <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -897,10 +899,10 @@
         <v>31</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -923,10 +925,10 @@
         <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -949,10 +951,10 @@
         <v>31</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -975,10 +977,10 @@
         <v>31</v>
       </c>
       <c r="I15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1001,10 +1003,10 @@
         <v>31</v>
       </c>
       <c r="I16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1027,10 +1029,10 @@
         <v>31</v>
       </c>
       <c r="I17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1053,10 +1055,10 @@
         <v>31</v>
       </c>
       <c r="I18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1079,10 +1081,10 @@
         <v>31</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1105,10 +1107,10 @@
         <v>31</v>
       </c>
       <c r="I20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1131,10 +1133,10 @@
         <v>31</v>
       </c>
       <c r="I21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1157,10 +1159,10 @@
         <v>31</v>
       </c>
       <c r="I22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1183,10 +1185,10 @@
         <v>31</v>
       </c>
       <c r="I23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1209,10 +1211,10 @@
         <v>31</v>
       </c>
       <c r="I24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1235,10 +1237,10 @@
         <v>31</v>
       </c>
       <c r="I25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1261,10 +1263,10 @@
         <v>31</v>
       </c>
       <c r="I26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1287,10 +1289,10 @@
         <v>31</v>
       </c>
       <c r="I27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1313,10 +1315,10 @@
         <v>31</v>
       </c>
       <c r="I28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1339,10 +1341,10 @@
         <v>31</v>
       </c>
       <c r="I29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1365,10 +1367,10 @@
         <v>31</v>
       </c>
       <c r="I30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1391,10 +1393,10 @@
         <v>31</v>
       </c>
       <c r="I31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1417,10 +1419,10 @@
         <v>31</v>
       </c>
       <c r="I32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1443,10 +1445,10 @@
         <v>31</v>
       </c>
       <c r="I33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1469,10 +1471,10 @@
         <v>31</v>
       </c>
       <c r="I34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1495,10 +1497,10 @@
         <v>31</v>
       </c>
       <c r="I35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1521,10 +1523,10 @@
         <v>31</v>
       </c>
       <c r="I36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1547,10 +1549,10 @@
         <v>31</v>
       </c>
       <c r="I37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1573,10 +1575,10 @@
         <v>31</v>
       </c>
       <c r="I38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -1599,10 +1601,10 @@
         <v>31</v>
       </c>
       <c r="I39" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -1625,10 +1627,10 @@
         <v>31</v>
       </c>
       <c r="I40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -1651,10 +1653,10 @@
         <v>31</v>
       </c>
       <c r="I41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1677,10 +1679,10 @@
         <v>31</v>
       </c>
       <c r="I42" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -1703,10 +1705,10 @@
         <v>31</v>
       </c>
       <c r="I43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1729,10 +1731,10 @@
         <v>31</v>
       </c>
       <c r="I44" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1755,10 +1757,10 @@
         <v>31</v>
       </c>
       <c r="I45" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1781,10 +1783,10 @@
         <v>31</v>
       </c>
       <c r="I46" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1807,10 +1809,10 @@
         <v>31</v>
       </c>
       <c r="I47" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1833,10 +1835,10 @@
         <v>31</v>
       </c>
       <c r="I48" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1859,10 +1861,10 @@
         <v>31</v>
       </c>
       <c r="I49" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -1885,10 +1887,10 @@
         <v>31</v>
       </c>
       <c r="I50" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -1911,10 +1913,10 @@
         <v>31</v>
       </c>
       <c r="I51" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -1937,10 +1939,10 @@
         <v>31</v>
       </c>
       <c r="I52" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -1963,10 +1965,10 @@
         <v>31</v>
       </c>
       <c r="I53" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -1989,10 +1991,10 @@
         <v>31</v>
       </c>
       <c r="I54" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -2015,10 +2017,10 @@
         <v>31</v>
       </c>
       <c r="I55" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2041,10 +2043,10 @@
         <v>31</v>
       </c>
       <c r="I56" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -2067,10 +2069,10 @@
         <v>31</v>
       </c>
       <c r="I57" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -2093,10 +2095,10 @@
         <v>31</v>
       </c>
       <c r="I58" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2119,10 +2121,10 @@
         <v>31</v>
       </c>
       <c r="I59" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -2145,10 +2147,10 @@
         <v>31</v>
       </c>
       <c r="I60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -2171,10 +2173,10 @@
         <v>31</v>
       </c>
       <c r="I61" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -2197,10 +2199,10 @@
         <v>31</v>
       </c>
       <c r="I62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -2223,10 +2225,10 @@
         <v>31</v>
       </c>
       <c r="I63" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>18</v>
       </c>
@@ -2249,10 +2251,10 @@
         <v>31</v>
       </c>
       <c r="I64" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -2275,10 +2277,10 @@
         <v>31</v>
       </c>
       <c r="I65" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -2301,10 +2303,10 @@
         <v>31</v>
       </c>
       <c r="I66" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -2327,10 +2329,10 @@
         <v>31</v>
       </c>
       <c r="I67" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -2353,10 +2355,10 @@
         <v>31</v>
       </c>
       <c r="I68" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -2379,10 +2381,10 @@
         <v>31</v>
       </c>
       <c r="I69" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -2405,10 +2407,10 @@
         <v>31</v>
       </c>
       <c r="I70" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -2431,10 +2433,10 @@
         <v>31</v>
       </c>
       <c r="I71" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>18</v>
       </c>
@@ -2457,10 +2459,10 @@
         <v>31</v>
       </c>
       <c r="I72" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -2483,10 +2485,10 @@
         <v>31</v>
       </c>
       <c r="I73" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -2509,10 +2511,10 @@
         <v>31</v>
       </c>
       <c r="I74" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>18</v>
       </c>
@@ -2535,10 +2537,10 @@
         <v>31</v>
       </c>
       <c r="I75" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>18</v>
       </c>
@@ -2561,10 +2563,10 @@
         <v>31</v>
       </c>
       <c r="I76" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -2587,10 +2589,10 @@
         <v>31</v>
       </c>
       <c r="I77" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>18</v>
       </c>
@@ -2613,10 +2615,10 @@
         <v>31</v>
       </c>
       <c r="I78" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -2639,10 +2641,10 @@
         <v>31</v>
       </c>
       <c r="I79" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -2665,10 +2667,10 @@
         <v>31</v>
       </c>
       <c r="I80" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>18</v>
       </c>
@@ -2691,10 +2693,10 @@
         <v>31</v>
       </c>
       <c r="I81" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>18</v>
       </c>
@@ -2717,10 +2719,10 @@
         <v>31</v>
       </c>
       <c r="I82" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>18</v>
       </c>
@@ -2743,10 +2745,10 @@
         <v>31</v>
       </c>
       <c r="I83" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>18</v>
       </c>
@@ -2769,10 +2771,10 @@
         <v>31</v>
       </c>
       <c r="I84" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>18</v>
       </c>
@@ -2795,10 +2797,10 @@
         <v>31</v>
       </c>
       <c r="I85" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>18</v>
       </c>
@@ -2821,10 +2823,10 @@
         <v>31</v>
       </c>
       <c r="I86" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>18</v>
       </c>
@@ -2847,10 +2849,10 @@
         <v>31</v>
       </c>
       <c r="I87" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>18</v>
       </c>
@@ -2873,10 +2875,10 @@
         <v>31</v>
       </c>
       <c r="I88" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>18</v>
       </c>
@@ -2899,10 +2901,10 @@
         <v>31</v>
       </c>
       <c r="I89" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>18</v>
       </c>
@@ -2925,10 +2927,10 @@
         <v>31</v>
       </c>
       <c r="I90" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>18</v>
       </c>
@@ -2951,10 +2953,10 @@
         <v>31</v>
       </c>
       <c r="I91" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -2977,10 +2979,10 @@
         <v>31</v>
       </c>
       <c r="I92" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>18</v>
       </c>
@@ -3003,10 +3005,10 @@
         <v>31</v>
       </c>
       <c r="I93" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>18</v>
       </c>
@@ -3029,10 +3031,10 @@
         <v>31</v>
       </c>
       <c r="I94" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>18</v>
       </c>
@@ -3055,10 +3057,10 @@
         <v>31</v>
       </c>
       <c r="I95" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -3081,10 +3083,10 @@
         <v>31</v>
       </c>
       <c r="I96" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>18</v>
       </c>
@@ -3107,10 +3109,10 @@
         <v>31</v>
       </c>
       <c r="I97" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>18</v>
       </c>
@@ -3133,10 +3135,10 @@
         <v>31</v>
       </c>
       <c r="I98" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>18</v>
       </c>
@@ -3159,10 +3161,10 @@
         <v>31</v>
       </c>
       <c r="I99" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>18</v>
       </c>
@@ -3185,10 +3187,10 @@
         <v>31</v>
       </c>
       <c r="I100" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>17</v>
       </c>
@@ -3211,10 +3213,10 @@
         <v>31</v>
       </c>
       <c r="I101" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>17</v>
       </c>
@@ -3237,10 +3239,10 @@
         <v>31</v>
       </c>
       <c r="I102" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>18</v>
       </c>
@@ -3263,10 +3265,10 @@
         <v>31</v>
       </c>
       <c r="I103" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>18</v>
       </c>
@@ -3289,7 +3291,7 @@
         <v>31</v>
       </c>
       <c r="I104" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>